<commit_message>
Particle System layer not needed.
</commit_message>
<xml_diff>
--- a/CodeBreakdown.xlsx
+++ b/CodeBreakdown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC9D7E2-F3C3-C041-8C00-1487FD05EDBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E934F620-6B94-9746-8FFC-74D8FB5EF5AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12740" yWindow="2260" windowWidth="27420" windowHeight="21280" xr2:uid="{5F473FF9-918D-1F43-A9D6-6F4A2D3B77D0}"/>
   </bookViews>
@@ -522,7 +522,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Moved default shaders into common.
</commit_message>
<xml_diff>
--- a/CodeBreakdown.xlsx
+++ b/CodeBreakdown.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E934F620-6B94-9746-8FFC-74D8FB5EF5AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598DE3FE-84C3-2442-BE68-00CC7DC1126C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12740" yWindow="2260" windowWidth="27420" windowHeight="21280" xr2:uid="{5F473FF9-918D-1F43-A9D6-6F4A2D3B77D0}"/>
+    <workbookView xWindow="19260" yWindow="460" windowWidth="28120" windowHeight="27000" xr2:uid="{5F473FF9-918D-1F43-A9D6-6F4A2D3B77D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="32">
   <si>
     <t xml:space="preserve">C Header </t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Get this higher!</t>
+  </si>
+  <si>
+    <t>Feb 19 - 3.0</t>
   </si>
 </sst>
 </file>
@@ -519,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FAE55-4088-2441-8851-2462CB328D4A}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,9 +900,6 @@
       <c r="B24" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J24" s="6" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
@@ -920,6 +920,9 @@
       <c r="G25">
         <v>2012</v>
       </c>
+      <c r="J25" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
@@ -1029,7 +1032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>8</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>1220</v>
       </c>
     </row>
-    <row r="36" spans="2:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B36" s="6" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>3633</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>19</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>7</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>8</v>
       </c>
@@ -1157,7 +1160,7 @@
         <v>4526</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1180,7 @@
         <v>9088</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>9</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>59203</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>29</v>
       </c>
@@ -1194,7 +1197,180 @@
         <f>E27/E43</f>
         <v>0.42536695775551914</v>
       </c>
-      <c r="J44" t="s">
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47">
+        <v>5588</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48">
+        <v>21898</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>27486</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E55">
+        <v>3009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56">
+        <v>3728</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61">
+        <v>2480</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62">
+        <v>20085</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63">
+        <v>27955</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65">
+        <f>E49+E56+E63</f>
+        <v>59169</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="3">
+        <f>E49/E65</f>
+        <v>0.46453379303351416</v>
+      </c>
+      <c r="J66" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
So close to 50!
</commit_message>
<xml_diff>
--- a/CodeBreakdown.xlsx
+++ b/CodeBreakdown.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjg/dev/WhirlyGlobe-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCA8DD0-8222-0B4A-95AD-6B3549EC25B5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5309F4D-EB4A-E84B-A534-0109F98719E0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="460" windowWidth="28120" windowHeight="20080" xr2:uid="{5F473FF9-918D-1F43-A9D6-6F4A2D3B77D0}"/>
+    <workbookView xWindow="3840" yWindow="460" windowWidth="30100" windowHeight="26740" xr2:uid="{5F473FF9-918D-1F43-A9D6-6F4A2D3B77D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="33">
   <si>
     <t xml:space="preserve">C Header </t>
   </si>
@@ -126,6 +127,9 @@
   </si>
   <si>
     <t>Feb 19 - 3.0</t>
+  </si>
+  <si>
+    <t>Feb 22 - 3.0</t>
   </si>
 </sst>
 </file>
@@ -522,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962FAE55-4088-2441-8851-2462CB328D4A}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,6 +1225,9 @@
       <c r="E47">
         <v>28054</v>
       </c>
+      <c r="J47" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
@@ -1287,7 +1294,100 @@
         <f>E47/E55</f>
         <v>0.47416546944984367</v>
       </c>
-      <c r="J56" t="s">
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60">
+        <v>29367</v>
+      </c>
+      <c r="J60" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63">
+        <v>3732</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66">
+        <v>26645</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68">
+        <f>E60+E63+E66</f>
+        <v>59744</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="E69" s="3">
+        <f>E60/E68</f>
+        <v>0.49154726834493839</v>
+      </c>
+      <c r="J69" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>